<commit_message>
Some small optimization and update documentation
</commit_message>
<xml_diff>
--- a/documentation/Planification initiale.xlsx
+++ b/documentation/Planification initiale.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Pre-TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christophe.KUNZLI\source\repos\Gestionnaire-TPI\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DC0666-E3DD-4F9A-9034-BA83AB3B179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C31EF7F-22BB-472A-A225-97089E7D3BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -962,9 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
done writing inital planning
</commit_message>
<xml_diff>
--- a/documentation/Planification initiale.xlsx
+++ b/documentation/Planification initiale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christophe.KUNZLI\source\repos\Gestionnaire-TPI\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C31EF7F-22BB-472A-A225-97089E7D3BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C6F02-0ED3-4FAF-A5C0-BB965D0FFEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19170" yWindow="5430" windowWidth="19425" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="par jours" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Semaine</t>
   </si>
@@ -159,6 +159,54 @@
   </si>
   <si>
     <t>Implémenter et tester la modification des données d'un TPI /pré-TPI</t>
+  </si>
+  <si>
+    <t>Documenter le travail de la semaine et se préparer pour la  semaine 6 si nécessaire</t>
+  </si>
+  <si>
+    <t>Se familliariser avec les dataGridView</t>
+  </si>
+  <si>
+    <t>Implémenter le formulaire permettant de saisir les informations pour créer un nouveau TPI</t>
+  </si>
+  <si>
+    <t>Implémenter la vérification de l'intégrité des données saisies</t>
+  </si>
+  <si>
+    <t>Documenter le travail de la semaine et se préparer pour la  semaine7 si nécessaire</t>
+  </si>
+  <si>
+    <t>Implémenter l'insertion du TPI saisi dans la DB</t>
+  </si>
+  <si>
+    <t>Ajouter au formulaire une liste de technologies qui peuvent être reliées au TPI ET modifier la requête d'ajout en conséquence</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Rendu du projet</t>
+  </si>
+  <si>
+    <t>Finalisation documentation</t>
+  </si>
+  <si>
+    <t>Préparation de la défense</t>
+  </si>
+  <si>
+    <t>Implémenter le bouton permettant de supprimmer un TPI</t>
+  </si>
+  <si>
+    <t>Implémenter un formulaire permettant de modifer les données d'un TPI existant</t>
+  </si>
+  <si>
+    <t>Documenter le travail de la semaine et se préparer pour la  semaine8 si nécessaire</t>
+  </si>
+  <si>
+    <t>Implémenter la vérification des données saisies</t>
+  </si>
+  <si>
+    <t>Implémenter la modification des données du TPI dans la DB</t>
   </si>
 </sst>
 </file>
@@ -509,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4654961-B0CA-4F38-AEFE-D4138AE20394}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,6 +834,9 @@
       <c r="C19" s="6">
         <v>2</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -797,6 +848,9 @@
       <c r="C20" s="6">
         <v>3</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -808,145 +862,226 @@
       <c r="C21" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>6</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="7">
+        <v>44999</v>
+      </c>
       <c r="C22" s="6">
         <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>6</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="7">
+        <v>45000</v>
+      </c>
       <c r="C23" s="6">
         <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>6</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7">
+        <v>45000</v>
+      </c>
       <c r="C24" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>6</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7">
+        <v>45001</v>
+      </c>
       <c r="C25" s="6">
         <v>3</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>6</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="7">
+        <v>45001</v>
+      </c>
       <c r="C26" s="6">
         <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>7</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="7">
+        <v>45006</v>
+      </c>
       <c r="C27" s="6">
         <v>3</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>7</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7">
+        <v>45007</v>
+      </c>
       <c r="C28" s="6">
         <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>7</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="7">
+        <v>45007</v>
+      </c>
       <c r="C29" s="6">
         <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>7</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7">
+        <v>45008</v>
+      </c>
       <c r="C30" s="6">
         <v>3</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>7</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7">
+        <v>45008</v>
+      </c>
       <c r="C31" s="6">
         <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>8</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7">
+        <v>45013</v>
+      </c>
       <c r="C32" s="6">
         <v>3</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>8</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7">
+        <v>45014</v>
+      </c>
       <c r="C33" s="6">
         <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>8</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="7">
+        <v>45014</v>
+      </c>
       <c r="C34" s="6">
         <v>2</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>8</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="7">
+        <v>45015</v>
+      </c>
       <c r="C35" s="6">
         <v>3</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>8</v>
       </c>
-      <c r="B36" s="7"/>
+      <c r="B36" s="7">
+        <v>45015</v>
+      </c>
       <c r="C36" s="6">
         <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>9</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>27</v>
@@ -962,7 +1097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>